<commit_message>
dagelijkse updates en project code toegevoegd
</commit_message>
<xml_diff>
--- a/Algemeen/Planning.xlsx
+++ b/Algemeen/Planning.xlsx
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Week</t>
   </si>
@@ -162,6 +162,18 @@
   </si>
   <si>
     <t>Dump files vergelijken</t>
+  </si>
+  <si>
+    <t>Kort voortgang gesprek met Peter</t>
+  </si>
+  <si>
+    <t>Met hond naar dierenarts</t>
+  </si>
+  <si>
+    <t>Vrij</t>
+  </si>
+  <si>
+    <t>Lang weekend weg</t>
   </si>
 </sst>
 </file>
@@ -218,7 +230,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -234,6 +246,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -347,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -362,6 +386,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -398,10 +423,19 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -708,7 +742,7 @@
   <dimension ref="A1:V30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12:R12"/>
+      <selection activeCell="J11" sqref="J11:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,15 +751,15 @@
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="13" t="s">
+      <c r="D1" s="18"/>
+      <c r="E1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
@@ -739,33 +773,33 @@
       <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20" t="s">
+      <c r="E2" s="21"/>
+      <c r="F2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20" t="s">
+      <c r="G2" s="21"/>
+      <c r="H2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20" t="s">
+      <c r="I2" s="21"/>
+      <c r="J2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20" t="s">
+      <c r="K2" s="21"/>
+      <c r="L2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20" t="s">
+      <c r="M2" s="21"/>
+      <c r="N2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -777,27 +811,27 @@
       <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22" t="s">
+      <c r="D3" s="22"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22" t="s">
+      <c r="G3" s="23"/>
+      <c r="H3" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="12" t="s">
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="15"/>
       <c r="T3" s="10"/>
       <c r="U3" t="s">
         <v>21</v>
@@ -813,27 +847,29 @@
       <c r="C4" s="3">
         <v>2</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="23" t="s">
+      <c r="E4" s="23"/>
+      <c r="F4" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="23"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="12" t="s">
+      <c r="G4" s="24"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" s="23"/>
+      <c r="N4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="15"/>
       <c r="T4" s="11"/>
       <c r="U4" t="s">
         <v>22</v>
@@ -849,23 +885,29 @@
       <c r="C5" s="3">
         <v>3</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="12" t="s">
+      <c r="D5" s="22"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="25"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="15"/>
+      <c r="T5" s="12"/>
+      <c r="U5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -877,21 +919,21 @@
       <c r="C6" s="3">
         <v>4</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="14"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="15"/>
       <c r="T6" s="7"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -904,23 +946,23 @@
       <c r="C7" s="3">
         <v>5</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="12" t="s">
+      <c r="D7" s="19"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="15"/>
       <c r="U7" s="7"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -933,23 +975,23 @@
       <c r="C8" s="3">
         <v>6</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="12" t="s">
+      <c r="D8" s="19"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="15"/>
       <c r="T8" s="7"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -962,23 +1004,23 @@
       <c r="C9" s="3">
         <v>7</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="12" t="s">
+      <c r="D9" s="26"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="15"/>
       <c r="U9" s="7"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
@@ -991,21 +1033,21 @@
       <c r="C10" s="3">
         <v>8</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="14"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="15"/>
       <c r="U10" s="7"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -1018,23 +1060,23 @@
       <c r="C11" s="3">
         <v>9</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="12" t="s">
+      <c r="D11" s="19"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="15"/>
       <c r="U11" s="7"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -1047,21 +1089,21 @@
       <c r="C12" s="3">
         <v>10</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="14"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="15"/>
       <c r="T12" s="7"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
@@ -1074,21 +1116,21 @@
       <c r="C13" s="3">
         <v>11</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="14"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="15"/>
       <c r="U13" s="7"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -1101,23 +1143,25 @@
       <c r="C14" s="3">
         <v>12</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
-      <c r="N14" s="12" t="s">
+      <c r="D14" s="19"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="M14" s="25"/>
+      <c r="N14" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="13"/>
-      <c r="R14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="15"/>
       <c r="V14" s="7"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
@@ -1130,23 +1174,25 @@
       <c r="C15" s="3">
         <v>13</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19"/>
-      <c r="N15" s="12" t="s">
+      <c r="D15" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="25"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="13"/>
-      <c r="R15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="15"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -1158,23 +1204,23 @@
       <c r="C16" s="3">
         <v>14</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="12" t="s">
+      <c r="D16" s="19"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="O16" s="13"/>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="13"/>
-      <c r="R16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="15"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -1186,23 +1232,23 @@
       <c r="C17" s="3">
         <v>15</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="12" t="s">
+      <c r="D17" s="19"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="13"/>
-      <c r="R17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="15"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
@@ -1214,23 +1260,23 @@
       <c r="C18" s="3">
         <v>16</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="12" t="s">
+      <c r="D18" s="19"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="13"/>
-      <c r="R18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="15"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -1242,21 +1288,21 @@
       <c r="C19" s="3">
         <v>17</v>
       </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="13"/>
-      <c r="R19" s="14"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="15"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
@@ -1268,21 +1314,21 @@
       <c r="C20" s="3">
         <v>18</v>
       </c>
-      <c r="D20" s="24"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="25"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="12"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
-      <c r="R20" s="14"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="15"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
@@ -1294,21 +1340,21 @@
       <c r="C21" s="3">
         <v>19</v>
       </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="12"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="13"/>
-      <c r="R21" s="14"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="15"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
@@ -1320,21 +1366,21 @@
       <c r="C22" s="3">
         <v>20</v>
       </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="12"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="13"/>
-      <c r="R22" s="14"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="14"/>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="15"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -1346,21 +1392,21 @@
       <c r="C23" s="3">
         <v>21</v>
       </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="12"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="13"/>
-      <c r="R23" s="14"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="14"/>
+      <c r="P23" s="14"/>
+      <c r="Q23" s="14"/>
+      <c r="R23" s="15"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
@@ -1372,21 +1418,21 @@
       <c r="C24" s="3">
         <v>22</v>
       </c>
-      <c r="D24" s="15"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="16"/>
-      <c r="N24" s="12"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="13"/>
-      <c r="Q24" s="13"/>
-      <c r="R24" s="14"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="14"/>
+      <c r="P24" s="14"/>
+      <c r="Q24" s="14"/>
+      <c r="R24" s="15"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
@@ -1398,21 +1444,21 @@
       <c r="C25" s="9">
         <v>23</v>
       </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="12"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="13"/>
-      <c r="Q25" s="13"/>
-      <c r="R25" s="14"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="20"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="14"/>
+      <c r="P25" s="14"/>
+      <c r="Q25" s="14"/>
+      <c r="R25" s="15"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
@@ -1424,21 +1470,21 @@
       <c r="C26" s="9">
         <v>24</v>
       </c>
-      <c r="D26" s="15"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="16"/>
-      <c r="N26" s="12"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="13"/>
-      <c r="Q26" s="13"/>
-      <c r="R26" s="14"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="14"/>
+      <c r="P26" s="14"/>
+      <c r="Q26" s="14"/>
+      <c r="R26" s="15"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
@@ -1450,21 +1496,21 @@
       <c r="C27" s="9">
         <v>25</v>
       </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19"/>
-      <c r="M27" s="19"/>
-      <c r="N27" s="12"/>
-      <c r="O27" s="13"/>
-      <c r="P27" s="13"/>
-      <c r="Q27" s="13"/>
-      <c r="R27" s="14"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="14"/>
+      <c r="P27" s="14"/>
+      <c r="Q27" s="14"/>
+      <c r="R27" s="15"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
@@ -1476,21 +1522,21 @@
       <c r="C28" s="9">
         <v>26</v>
       </c>
-      <c r="D28" s="15"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16"/>
-      <c r="L28" s="16"/>
-      <c r="M28" s="16"/>
-      <c r="N28" s="12"/>
-      <c r="O28" s="13"/>
-      <c r="P28" s="13"/>
-      <c r="Q28" s="13"/>
-      <c r="R28" s="14"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="14"/>
+      <c r="P28" s="14"/>
+      <c r="Q28" s="14"/>
+      <c r="R28" s="15"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
@@ -1502,38 +1548,38 @@
       <c r="C29" s="9">
         <v>27</v>
       </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="19"/>
-      <c r="L29" s="19"/>
-      <c r="M29" s="19"/>
-      <c r="N29" s="12"/>
-      <c r="O29" s="13"/>
-      <c r="P29" s="13"/>
-      <c r="Q29" s="13"/>
-      <c r="R29" s="14"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="14"/>
+      <c r="P29" s="14"/>
+      <c r="Q29" s="14"/>
+      <c r="R29" s="15"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D30" s="15"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="16"/>
-      <c r="L30" s="16"/>
-      <c r="M30" s="16"/>
-      <c r="N30" s="12"/>
-      <c r="O30" s="13"/>
-      <c r="P30" s="13"/>
-      <c r="Q30" s="13"/>
-      <c r="R30" s="14"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="14"/>
+      <c r="P30" s="14"/>
+      <c r="Q30" s="14"/>
+      <c r="R30" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="176">

</xml_diff>

<commit_message>
update source code en planning
</commit_message>
<xml_diff>
--- a/Algemeen/Planning.xlsx
+++ b/Algemeen/Planning.xlsx
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>Week</t>
   </si>
@@ -104,9 +104,6 @@
     <t>Vrijdag</t>
   </si>
   <si>
-    <t>Opmerking week</t>
-  </si>
-  <si>
     <t>Schrijven</t>
   </si>
   <si>
@@ -140,12 +137,6 @@
     <t>Logboek implementeren</t>
   </si>
   <si>
-    <t>Aanwezig</t>
-  </si>
-  <si>
-    <t>Afwezig</t>
-  </si>
-  <si>
     <t>Stageovereenkomst ingeleverd</t>
   </si>
   <si>
@@ -170,10 +161,52 @@
     <t>Met hond naar dierenarts</t>
   </si>
   <si>
-    <t>Vrij</t>
-  </si>
-  <si>
     <t>Lang weekend weg</t>
+  </si>
+  <si>
+    <t>Thuis gewerkt; Kristina ziek -&gt; naar doctor</t>
+  </si>
+  <si>
+    <t>Gewerkt aanwezig</t>
+  </si>
+  <si>
+    <t>Gewerkt afwezig/ziek</t>
+  </si>
+  <si>
+    <t>Niet gewerkt - vrij</t>
+  </si>
+  <si>
+    <t>Elke 10e werkdag</t>
+  </si>
+  <si>
+    <t>100 Werkdagen</t>
+  </si>
+  <si>
+    <t>Aantal niet gewerkte werkdagen inhalen</t>
+  </si>
+  <si>
+    <t>W3D3</t>
+  </si>
+  <si>
+    <t>W12D5</t>
+  </si>
+  <si>
+    <t>W13D1</t>
+  </si>
+  <si>
+    <t>(Week / Dag)</t>
+  </si>
+  <si>
+    <t>Opmerking week / planning</t>
+  </si>
+  <si>
+    <t>W11D4</t>
+  </si>
+  <si>
+    <t>W11D5</t>
+  </si>
+  <si>
+    <t>Online spel release</t>
   </si>
 </sst>
 </file>
@@ -230,7 +263,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -261,8 +294,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -367,11 +406,147 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -387,28 +562,47 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -426,6 +620,12 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -435,8 +635,41 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -739,10 +972,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V30"/>
+  <dimension ref="A1:V28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11:K11"/>
+      <selection activeCell="N14" sqref="N14:R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,14 +985,14 @@
         <v>3</v>
       </c>
       <c r="C1" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="18"/>
+      <c r="E1" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
@@ -773,33 +1006,33 @@
       <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21" t="s">
+      <c r="E2" s="30"/>
+      <c r="F2" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21" t="s">
+      <c r="G2" s="30"/>
+      <c r="H2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21" t="s">
+      <c r="I2" s="30"/>
+      <c r="J2" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21" t="s">
+      <c r="K2" s="30"/>
+      <c r="L2" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -811,30 +1044,30 @@
       <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="15"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="24"/>
       <c r="T3" s="10"/>
       <c r="U3" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -847,32 +1080,32 @@
       <c r="C4" s="3">
         <v>2</v>
       </c>
-      <c r="D4" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="24"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="23"/>
-      <c r="N4" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="15"/>
+      <c r="D4" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="32"/>
+      <c r="F4" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="33"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="32"/>
+      <c r="N4" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="24"/>
       <c r="T4" s="11"/>
       <c r="U4" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -885,28 +1118,28 @@
       <c r="C5" s="3">
         <v>3</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="25"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="15"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="34"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="24"/>
       <c r="T5" s="12"/>
       <c r="U5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -919,22 +1152,27 @@
       <c r="C6" s="3">
         <v>4</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="15"/>
-      <c r="T6" s="7"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="33"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="24"/>
+      <c r="T6" s="14"/>
+      <c r="U6" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -943,26 +1181,26 @@
       <c r="B7" s="1">
         <v>41915</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="13">
         <v>5</v>
       </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="15"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="24"/>
       <c r="U7" s="7"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -975,23 +1213,23 @@
       <c r="C8" s="3">
         <v>6</v>
       </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="15"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="24"/>
       <c r="T8" s="7"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -1004,23 +1242,23 @@
       <c r="C9" s="3">
         <v>7</v>
       </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="15"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="24"/>
       <c r="U9" s="7"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
@@ -1033,21 +1271,21 @@
       <c r="C10" s="3">
         <v>8</v>
       </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="15"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="24"/>
       <c r="U10" s="7"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -1060,23 +1298,23 @@
       <c r="C11" s="3">
         <v>9</v>
       </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="15"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="24"/>
       <c r="U11" s="7"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -1089,21 +1327,21 @@
       <c r="C12" s="3">
         <v>10</v>
       </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="15"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="24"/>
       <c r="T12" s="7"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
@@ -1116,21 +1354,23 @@
       <c r="C13" s="3">
         <v>11</v>
       </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="15"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="K13" s="50"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="51"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="24"/>
       <c r="U13" s="7"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -1143,25 +1383,25 @@
       <c r="C14" s="3">
         <v>12</v>
       </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="M14" s="25"/>
-      <c r="N14" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="15"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="M14" s="34"/>
+      <c r="N14" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="O14" s="19"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="24"/>
       <c r="V14" s="7"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
@@ -1174,25 +1414,25 @@
       <c r="C15" s="3">
         <v>13</v>
       </c>
-      <c r="D15" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="25"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="15"/>
+      <c r="D15" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="34"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="O15" s="19"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="24"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -1204,23 +1444,23 @@
       <c r="C16" s="3">
         <v>14</v>
       </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="15"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="24"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -1232,23 +1472,23 @@
       <c r="C17" s="3">
         <v>15</v>
       </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="15"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="O17" s="19"/>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="24"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
@@ -1260,23 +1500,23 @@
       <c r="C18" s="3">
         <v>16</v>
       </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="14"/>
-      <c r="R18" s="15"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26"/>
+      <c r="N18" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="O18" s="19"/>
+      <c r="P18" s="19"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="24"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -1288,21 +1528,21 @@
       <c r="C19" s="3">
         <v>17</v>
       </c>
-      <c r="D19" s="26"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="27"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="29"/>
-      <c r="M19" s="29"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="15"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="43"/>
+      <c r="M19" s="43"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="24"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
@@ -1314,21 +1554,21 @@
       <c r="C20" s="3">
         <v>18</v>
       </c>
-      <c r="D20" s="26"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="27"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="15"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
+      <c r="Q20" s="19"/>
+      <c r="R20" s="24"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
@@ -1340,47 +1580,49 @@
       <c r="C21" s="3">
         <v>19</v>
       </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="15"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="D21" s="25"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="23"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="24"/>
+    </row>
+    <row r="22" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="15">
         <v>42016</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="15">
         <v>42020</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="16">
         <v>20</v>
       </c>
-      <c r="D22" s="19"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="14"/>
-      <c r="R22" s="15"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="41"/>
+      <c r="L22" s="41"/>
+      <c r="M22" s="42"/>
+      <c r="N22" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="O22" s="45"/>
+      <c r="P22" s="45"/>
+      <c r="Q22" s="45"/>
+      <c r="R22" s="46"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -1392,21 +1634,33 @@
       <c r="C23" s="3">
         <v>21</v>
       </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
-      <c r="M23" s="20"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="14"/>
-      <c r="P23" s="14"/>
-      <c r="Q23" s="14"/>
-      <c r="R23" s="15"/>
+      <c r="D23" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="K23" s="36"/>
+      <c r="L23" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="M23" s="36"/>
+      <c r="N23" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="O23" s="48"/>
+      <c r="P23" s="48"/>
+      <c r="Q23" s="48"/>
+      <c r="R23" s="49"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
@@ -1418,21 +1672,23 @@
       <c r="C24" s="3">
         <v>22</v>
       </c>
-      <c r="D24" s="16"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="17"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="14"/>
-      <c r="Q24" s="14"/>
-      <c r="R24" s="15"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="O24" s="21"/>
+      <c r="P24" s="21"/>
+      <c r="Q24" s="21"/>
+      <c r="R24" s="22"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
@@ -1444,21 +1700,21 @@
       <c r="C25" s="9">
         <v>23</v>
       </c>
-      <c r="D25" s="19"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20"/>
-      <c r="M25" s="20"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="14"/>
-      <c r="P25" s="14"/>
-      <c r="Q25" s="14"/>
-      <c r="R25" s="15"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="19"/>
+      <c r="Q25" s="19"/>
+      <c r="R25" s="24"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
@@ -1470,21 +1726,21 @@
       <c r="C26" s="9">
         <v>24</v>
       </c>
-      <c r="D26" s="16"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="14"/>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="15"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="29"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="19"/>
+      <c r="R26" s="24"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
@@ -1496,21 +1752,21 @@
       <c r="C27" s="9">
         <v>25</v>
       </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="15"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="26"/>
+      <c r="M27" s="26"/>
+      <c r="N27" s="23"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="24"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
@@ -1519,70 +1775,27 @@
       <c r="B28" s="8">
         <v>42062</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="17">
         <v>26</v>
       </c>
-      <c r="D28" s="16"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="14"/>
-      <c r="R28" s="15"/>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="6">
-        <v>42065</v>
-      </c>
-      <c r="B29" s="8">
-        <v>42069</v>
-      </c>
-      <c r="C29" s="9">
-        <v>27</v>
-      </c>
-      <c r="D29" s="19"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="20"/>
-      <c r="L29" s="20"/>
-      <c r="M29" s="20"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="14"/>
-      <c r="P29" s="14"/>
-      <c r="Q29" s="14"/>
-      <c r="R29" s="15"/>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D30" s="16"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17"/>
-      <c r="M30" s="17"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="14"/>
-      <c r="P30" s="14"/>
-      <c r="Q30" s="14"/>
-      <c r="R30" s="15"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="26"/>
+      <c r="M28" s="27"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="19"/>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="176">
+  <mergeCells count="163">
     <mergeCell ref="N22:R22"/>
     <mergeCell ref="N23:R23"/>
     <mergeCell ref="N13:R13"/>
@@ -1668,8 +1881,7 @@
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="J13:M13"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="H10:I10"/>
@@ -1690,7 +1902,6 @@
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:M9"/>
-    <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="J6:K6"/>
@@ -1700,6 +1911,19 @@
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="L7:M7"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="H4:I4"/>
@@ -1710,16 +1934,19 @@
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="L5:M5"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="N24:R24"/>
+    <mergeCell ref="N25:R25"/>
+    <mergeCell ref="N26:R26"/>
+    <mergeCell ref="N27:R27"/>
+    <mergeCell ref="N28:R28"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="L27:M27"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="F28:G28"/>
     <mergeCell ref="H28:I28"/>
@@ -1732,33 +1959,6 @@
     <mergeCell ref="L25:M25"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="F26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="N30:R30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="N24:R24"/>
-    <mergeCell ref="N25:R25"/>
-    <mergeCell ref="N26:R26"/>
-    <mergeCell ref="N27:R27"/>
-    <mergeCell ref="N28:R28"/>
-    <mergeCell ref="N29:R29"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="L27:M27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
directories fixen en update
</commit_message>
<xml_diff>
--- a/Algemeen/Planning.xlsx
+++ b/Algemeen/Planning.xlsx
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>Week</t>
   </si>
@@ -174,9 +174,6 @@
   </si>
   <si>
     <t>Niet gewerkt - vrij</t>
-  </si>
-  <si>
-    <t>Elke 10e werkdag</t>
   </si>
   <si>
     <t>100 Werkdagen</t>
@@ -263,7 +260,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -294,14 +291,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -542,11 +533,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -561,14 +565,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -620,6 +625,12 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -631,6 +642,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -664,12 +681,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -975,7 +986,7 @@
   <dimension ref="A1:V28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14:R14"/>
+      <selection activeCell="F24" sqref="F24:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,15 +995,15 @@
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="19" t="s">
+      <c r="D1" s="19"/>
+      <c r="E1" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
@@ -1006,33 +1017,33 @@
       <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30" t="s">
+      <c r="E2" s="31"/>
+      <c r="F2" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30" t="s">
+      <c r="G2" s="31"/>
+      <c r="H2" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30" t="s">
+      <c r="I2" s="31"/>
+      <c r="J2" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30" t="s">
+      <c r="K2" s="31"/>
+      <c r="L2" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -1044,27 +1055,27 @@
       <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32" t="s">
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32" t="s">
+      <c r="G3" s="33"/>
+      <c r="H3" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="23" t="s">
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="24"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="25"/>
       <c r="T3" s="10"/>
       <c r="U3" t="s">
         <v>30</v>
@@ -1080,29 +1091,29 @@
       <c r="C4" s="3">
         <v>2</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="32"/>
-      <c r="F4" s="33" t="s">
+      <c r="E4" s="33"/>
+      <c r="F4" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="33"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32" t="s">
+      <c r="G4" s="34"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="32"/>
-      <c r="N4" s="23" t="s">
+      <c r="M4" s="33"/>
+      <c r="N4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="24"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="25"/>
       <c r="T4" s="11"/>
       <c r="U4" t="s">
         <v>31</v>
@@ -1118,26 +1129,26 @@
       <c r="C5" s="3">
         <v>3</v>
       </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="34" t="s">
+      <c r="D5" s="32"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="34"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="23" t="s">
+      <c r="I5" s="35"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="24"/>
-      <c r="T5" s="12"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="25"/>
+      <c r="T5" s="17"/>
       <c r="U5" t="s">
         <v>32</v>
       </c>
@@ -1152,27 +1163,26 @@
       <c r="C6" s="3">
         <v>4</v>
       </c>
-      <c r="D6" s="31"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="33" t="s">
+      <c r="D6" s="32"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="33"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="19"/>
-      <c r="R6" s="24"/>
-      <c r="T6" s="14"/>
-      <c r="U6" t="s">
-        <v>33</v>
-      </c>
+      <c r="G6" s="34"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="25"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -1181,26 +1191,26 @@
       <c r="B7" s="1">
         <v>41915</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="12">
         <v>5</v>
       </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="23" t="s">
+      <c r="D7" s="36"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="19"/>
-      <c r="R7" s="24"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="25"/>
       <c r="U7" s="7"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -1213,23 +1223,23 @@
       <c r="C8" s="3">
         <v>6</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="23" t="s">
+      <c r="D8" s="38"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="19"/>
-      <c r="R8" s="24"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="25"/>
       <c r="T8" s="7"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -1242,23 +1252,23 @@
       <c r="C9" s="3">
         <v>7</v>
       </c>
-      <c r="D9" s="37"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="38"/>
-      <c r="M9" s="38"/>
-      <c r="N9" s="23" t="s">
+      <c r="D9" s="40"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="41"/>
+      <c r="N9" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="24"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="25"/>
       <c r="U9" s="7"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
@@ -1271,21 +1281,21 @@
       <c r="C10" s="3">
         <v>8</v>
       </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="24"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="25"/>
       <c r="U10" s="7"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -1298,23 +1308,23 @@
       <c r="C11" s="3">
         <v>9</v>
       </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="23" t="s">
+      <c r="D11" s="26"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="24"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="25"/>
       <c r="U11" s="7"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -1327,21 +1337,21 @@
       <c r="C12" s="3">
         <v>10</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="24"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="25"/>
       <c r="T12" s="7"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
@@ -1354,23 +1364,23 @@
       <c r="C13" s="3">
         <v>11</v>
       </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="K13" s="50"/>
-      <c r="L13" s="50"/>
-      <c r="M13" s="51"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="19"/>
-      <c r="Q13" s="19"/>
-      <c r="R13" s="24"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="K13" s="42"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="24"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="25"/>
       <c r="U13" s="7"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -1383,25 +1393,25 @@
       <c r="C14" s="3">
         <v>12</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="34" t="s">
+      <c r="D14" s="26"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="M14" s="34"/>
-      <c r="N14" s="23" t="s">
+      <c r="M14" s="35"/>
+      <c r="N14" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="O14" s="19"/>
-      <c r="P14" s="19"/>
-      <c r="Q14" s="19"/>
-      <c r="R14" s="24"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="25"/>
       <c r="V14" s="7"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
@@ -1414,25 +1424,25 @@
       <c r="C15" s="3">
         <v>13</v>
       </c>
-      <c r="D15" s="39" t="s">
+      <c r="D15" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="34"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="23" t="s">
+      <c r="E15" s="35"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="O15" s="19"/>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="19"/>
-      <c r="R15" s="24"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="25"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -1444,23 +1454,23 @@
       <c r="C16" s="3">
         <v>14</v>
       </c>
-      <c r="D16" s="25"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="23" t="s">
+      <c r="D16" s="26"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="O16" s="19"/>
-      <c r="P16" s="19"/>
-      <c r="Q16" s="19"/>
-      <c r="R16" s="24"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="25"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -1472,23 +1482,23 @@
       <c r="C17" s="3">
         <v>15</v>
       </c>
-      <c r="D17" s="25"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="23" t="s">
+      <c r="D17" s="26"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="O17" s="19"/>
-      <c r="P17" s="19"/>
-      <c r="Q17" s="19"/>
-      <c r="R17" s="24"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="25"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
@@ -1500,23 +1510,23 @@
       <c r="C18" s="3">
         <v>16</v>
       </c>
-      <c r="D18" s="25"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="26"/>
-      <c r="N18" s="23" t="s">
+      <c r="D18" s="26"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="O18" s="19"/>
-      <c r="P18" s="19"/>
-      <c r="Q18" s="19"/>
-      <c r="R18" s="24"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="25"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -1528,21 +1538,21 @@
       <c r="C19" s="3">
         <v>17</v>
       </c>
-      <c r="D19" s="37"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="38"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="43"/>
-      <c r="N19" s="23"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="19"/>
-      <c r="Q19" s="19"/>
-      <c r="R19" s="24"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="41"/>
+      <c r="L19" s="48"/>
+      <c r="M19" s="48"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="20"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="20"/>
+      <c r="R19" s="25"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
@@ -1554,21 +1564,21 @@
       <c r="C20" s="3">
         <v>18</v>
       </c>
-      <c r="D20" s="37"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="38"/>
-      <c r="M20" s="38"/>
-      <c r="N20" s="23"/>
-      <c r="O20" s="19"/>
-      <c r="P20" s="19"/>
-      <c r="Q20" s="19"/>
-      <c r="R20" s="24"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="41"/>
+      <c r="L20" s="41"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="24"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="20"/>
+      <c r="R20" s="25"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
@@ -1580,49 +1590,49 @@
       <c r="C21" s="3">
         <v>19</v>
       </c>
-      <c r="D21" s="25"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="23"/>
-      <c r="O21" s="19"/>
-      <c r="P21" s="19"/>
-      <c r="Q21" s="19"/>
-      <c r="R21" s="24"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="24"/>
+      <c r="O21" s="20"/>
+      <c r="P21" s="20"/>
+      <c r="Q21" s="20"/>
+      <c r="R21" s="25"/>
     </row>
     <row r="22" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="15">
+      <c r="A22" s="13">
         <v>42016</v>
       </c>
-      <c r="B22" s="15">
+      <c r="B22" s="13">
         <v>42020</v>
       </c>
-      <c r="C22" s="16">
+      <c r="C22" s="14">
         <v>20</v>
       </c>
-      <c r="D22" s="40"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="41"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="41"/>
-      <c r="M22" s="42"/>
-      <c r="N22" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="O22" s="45"/>
-      <c r="P22" s="45"/>
-      <c r="Q22" s="45"/>
-      <c r="R22" s="46"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="47"/>
+      <c r="N22" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="O22" s="50"/>
+      <c r="P22" s="50"/>
+      <c r="Q22" s="50"/>
+      <c r="R22" s="51"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -1634,33 +1644,33 @@
       <c r="C23" s="3">
         <v>21</v>
       </c>
-      <c r="D23" s="35" t="s">
+      <c r="D23" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="I23" s="36"/>
-      <c r="J23" s="36" t="s">
+      <c r="K23" s="39"/>
+      <c r="L23" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="K23" s="36"/>
-      <c r="L23" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="M23" s="36"/>
-      <c r="N23" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="O23" s="48"/>
-      <c r="P23" s="48"/>
-      <c r="Q23" s="48"/>
-      <c r="R23" s="49"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="52" t="s">
+        <v>34</v>
+      </c>
+      <c r="O23" s="53"/>
+      <c r="P23" s="53"/>
+      <c r="Q23" s="53"/>
+      <c r="R23" s="54"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
@@ -1672,23 +1682,23 @@
       <c r="C24" s="3">
         <v>22</v>
       </c>
-      <c r="D24" s="28"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="29"/>
-      <c r="K24" s="29"/>
-      <c r="L24" s="29"/>
-      <c r="M24" s="29"/>
-      <c r="N24" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="O24" s="21"/>
-      <c r="P24" s="21"/>
-      <c r="Q24" s="21"/>
-      <c r="R24" s="22"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="O24" s="22"/>
+      <c r="P24" s="22"/>
+      <c r="Q24" s="22"/>
+      <c r="R24" s="23"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
@@ -1700,21 +1710,21 @@
       <c r="C25" s="9">
         <v>23</v>
       </c>
-      <c r="D25" s="25"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="26"/>
-      <c r="N25" s="23"/>
-      <c r="O25" s="19"/>
-      <c r="P25" s="19"/>
-      <c r="Q25" s="19"/>
-      <c r="R25" s="24"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="27"/>
+      <c r="M25" s="27"/>
+      <c r="N25" s="24"/>
+      <c r="O25" s="20"/>
+      <c r="P25" s="20"/>
+      <c r="Q25" s="20"/>
+      <c r="R25" s="25"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
@@ -1726,21 +1736,21 @@
       <c r="C26" s="9">
         <v>24</v>
       </c>
-      <c r="D26" s="28"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="29"/>
-      <c r="K26" s="29"/>
-      <c r="L26" s="29"/>
-      <c r="M26" s="29"/>
-      <c r="N26" s="23"/>
-      <c r="O26" s="19"/>
-      <c r="P26" s="19"/>
-      <c r="Q26" s="19"/>
-      <c r="R26" s="24"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="30"/>
+      <c r="N26" s="24"/>
+      <c r="O26" s="20"/>
+      <c r="P26" s="20"/>
+      <c r="Q26" s="20"/>
+      <c r="R26" s="25"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
@@ -1752,21 +1762,21 @@
       <c r="C27" s="9">
         <v>25</v>
       </c>
-      <c r="D27" s="25"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="26"/>
-      <c r="M27" s="26"/>
-      <c r="N27" s="23"/>
-      <c r="O27" s="19"/>
-      <c r="P27" s="19"/>
-      <c r="Q27" s="19"/>
-      <c r="R27" s="24"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="27"/>
+      <c r="L27" s="27"/>
+      <c r="M27" s="27"/>
+      <c r="N27" s="24"/>
+      <c r="O27" s="20"/>
+      <c r="P27" s="20"/>
+      <c r="Q27" s="20"/>
+      <c r="R27" s="25"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
@@ -1775,24 +1785,24 @@
       <c r="B28" s="8">
         <v>42062</v>
       </c>
-      <c r="C28" s="17">
+      <c r="C28" s="15">
         <v>26</v>
       </c>
-      <c r="D28" s="25"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="26"/>
-      <c r="M28" s="27"/>
-      <c r="N28" s="19"/>
-      <c r="O28" s="19"/>
-      <c r="P28" s="19"/>
-      <c r="Q28" s="19"/>
-      <c r="R28" s="24"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="27"/>
+      <c r="L28" s="27"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="20"/>
+      <c r="O28" s="20"/>
+      <c r="P28" s="20"/>
+      <c r="Q28" s="20"/>
+      <c r="R28" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="163">

</xml_diff>

<commit_message>
oude status met code vanaf 3okt, ivm linker problemen
</commit_message>
<xml_diff>
--- a/Algemeen/Planning.xlsx
+++ b/Algemeen/Planning.xlsx
@@ -70,12 +70,109 @@
         </r>
       </text>
     </comment>
+    <comment ref="C12" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Olivier:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Stagepresentatie op school?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Olivier:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Intervisie; conceptverslag stageverslag en reflectie</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Olivier:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Eindbeoordeling bedrijf
+(werk en inhoud verslag)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Olivier:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Beoordelen stageverslag</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>Week</t>
   </si>
@@ -161,9 +258,6 @@
     <t>Met hond naar dierenarts</t>
   </si>
   <si>
-    <t>Lang weekend weg</t>
-  </si>
-  <si>
     <t>Thuis gewerkt; Kristina ziek -&gt; naar doctor</t>
   </si>
   <si>
@@ -203,7 +297,7 @@
     <t>W11D5</t>
   </si>
   <si>
-    <t>Online spel release</t>
+    <t>Weekend weg</t>
   </si>
 </sst>
 </file>
@@ -550,7 +644,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -631,10 +725,10 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -649,8 +743,8 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -659,6 +753,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -985,8 +1085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24:G24"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,7 +1138,7 @@
       </c>
       <c r="M2" s="31"/>
       <c r="N2" s="31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O2" s="31"/>
       <c r="P2" s="31"/>
@@ -1078,7 +1178,7 @@
       <c r="R3" s="25"/>
       <c r="T3" s="10"/>
       <c r="U3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -1116,7 +1216,7 @@
       <c r="R4" s="25"/>
       <c r="T4" s="11"/>
       <c r="U4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -1150,7 +1250,7 @@
       <c r="R5" s="25"/>
       <c r="T5" s="17"/>
       <c r="U5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -1166,7 +1266,7 @@
       <c r="D6" s="32"/>
       <c r="E6" s="33"/>
       <c r="F6" s="34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6" s="34"/>
       <c r="H6" s="33"/>
@@ -1196,14 +1296,14 @@
       </c>
       <c r="D7" s="36"/>
       <c r="E7" s="37"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="27"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
       <c r="N7" s="24" t="s">
         <v>14</v>
       </c>
@@ -1371,7 +1471,7 @@
       <c r="H13" s="27"/>
       <c r="I13" s="27"/>
       <c r="J13" s="42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K13" s="42"/>
       <c r="L13" s="42"/>
@@ -1401,10 +1501,10 @@
       <c r="I14" s="27"/>
       <c r="J14" s="27"/>
       <c r="K14" s="27"/>
-      <c r="L14" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="M14" s="35"/>
+      <c r="L14" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="M14" s="43"/>
       <c r="N14" s="24" t="s">
         <v>19</v>
       </c>
@@ -1425,9 +1525,9 @@
         <v>13</v>
       </c>
       <c r="D15" s="44" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="35"/>
+        <v>41</v>
+      </c>
+      <c r="E15" s="42"/>
       <c r="F15" s="27"/>
       <c r="G15" s="27"/>
       <c r="H15" s="27"/>
@@ -1546,8 +1646,8 @@
       <c r="I19" s="41"/>
       <c r="J19" s="41"/>
       <c r="K19" s="41"/>
-      <c r="L19" s="48"/>
-      <c r="M19" s="48"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="50"/>
       <c r="N19" s="24"/>
       <c r="O19" s="20"/>
       <c r="P19" s="20"/>
@@ -1626,13 +1726,13 @@
       <c r="K22" s="46"/>
       <c r="L22" s="46"/>
       <c r="M22" s="47"/>
-      <c r="N22" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="O22" s="50"/>
-      <c r="P22" s="50"/>
-      <c r="Q22" s="50"/>
-      <c r="R22" s="51"/>
+      <c r="N22" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="O22" s="52"/>
+      <c r="P22" s="52"/>
+      <c r="Q22" s="52"/>
+      <c r="R22" s="53"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -1644,33 +1744,33 @@
       <c r="C23" s="3">
         <v>21</v>
       </c>
-      <c r="D23" s="38" t="s">
+      <c r="D23" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39" t="s">
+      <c r="K23" s="49"/>
+      <c r="L23" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="K23" s="39"/>
-      <c r="L23" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="M23" s="39"/>
-      <c r="N23" s="52" t="s">
-        <v>34</v>
-      </c>
-      <c r="O23" s="53"/>
-      <c r="P23" s="53"/>
-      <c r="Q23" s="53"/>
-      <c r="R23" s="54"/>
+      <c r="M23" s="49"/>
+      <c r="N23" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="O23" s="55"/>
+      <c r="P23" s="55"/>
+      <c r="Q23" s="55"/>
+      <c r="R23" s="56"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
@@ -1693,7 +1793,7 @@
       <c r="L24" s="30"/>
       <c r="M24" s="30"/>
       <c r="N24" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O24" s="22"/>
       <c r="P24" s="22"/>

</xml_diff>

<commit_message>
update met veel extra functies...
</commit_message>
<xml_diff>
--- a/Algemeen/Planning.xlsx
+++ b/Algemeen/Planning.xlsx
@@ -172,7 +172,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <t>Week</t>
   </si>
@@ -298,6 +298,9 @@
   </si>
   <si>
     <t>Weekend weg</t>
+  </si>
+  <si>
+    <t>Ziek; maag/keel</t>
   </si>
 </sst>
 </file>
@@ -668,10 +671,106 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -683,104 +782,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1086,7 +1089,7 @@
   <dimension ref="A1:V28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7:K7"/>
+      <selection activeCell="J13" sqref="J13:M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,15 +1098,15 @@
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="20" t="s">
+      <c r="D1" s="52"/>
+      <c r="E1" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
@@ -1117,33 +1120,33 @@
       <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31" t="s">
+      <c r="E2" s="33"/>
+      <c r="F2" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31" t="s">
+      <c r="G2" s="33"/>
+      <c r="H2" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31" t="s">
+      <c r="I2" s="33"/>
+      <c r="J2" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31" t="s">
+      <c r="K2" s="33"/>
+      <c r="L2" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31" t="s">
+      <c r="M2" s="33"/>
+      <c r="N2" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -1155,27 +1158,27 @@
       <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33" t="s">
+      <c r="D3" s="48"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33" t="s">
+      <c r="G3" s="46"/>
+      <c r="H3" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="24" t="s">
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="25"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="27"/>
       <c r="T3" s="10"/>
       <c r="U3" t="s">
         <v>29</v>
@@ -1191,29 +1194,29 @@
       <c r="C4" s="3">
         <v>2</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="33"/>
-      <c r="F4" s="34" t="s">
+      <c r="E4" s="46"/>
+      <c r="F4" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="34"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33" t="s">
+      <c r="G4" s="47"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="33"/>
-      <c r="N4" s="24" t="s">
+      <c r="M4" s="46"/>
+      <c r="N4" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="25"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="27"/>
       <c r="T4" s="11"/>
       <c r="U4" t="s">
         <v>30</v>
@@ -1229,25 +1232,25 @@
       <c r="C5" s="3">
         <v>3</v>
       </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="35" t="s">
+      <c r="D5" s="48"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="35"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="24" t="s">
+      <c r="I5" s="51"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="25"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="27"/>
       <c r="T5" s="17"/>
       <c r="U5" t="s">
         <v>31</v>
@@ -1263,23 +1266,23 @@
       <c r="C6" s="3">
         <v>4</v>
       </c>
-      <c r="D6" s="32"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="34" t="s">
+      <c r="D6" s="48"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="34"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="20"/>
-      <c r="P6" s="20"/>
-      <c r="Q6" s="20"/>
-      <c r="R6" s="25"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="27"/>
       <c r="T6" s="18"/>
       <c r="U6" s="16"/>
       <c r="V6" s="16"/>
@@ -1294,23 +1297,23 @@
       <c r="C7" s="12">
         <v>5</v>
       </c>
-      <c r="D7" s="36"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="24" t="s">
+      <c r="D7" s="49"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
+      <c r="N7" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="O7" s="20"/>
-      <c r="P7" s="20"/>
-      <c r="Q7" s="20"/>
-      <c r="R7" s="25"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26"/>
+      <c r="R7" s="27"/>
       <c r="U7" s="7"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -1323,23 +1326,25 @@
       <c r="C8" s="3">
         <v>6</v>
       </c>
-      <c r="D8" s="38"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="27"/>
-      <c r="N8" s="24" t="s">
+      <c r="D8" s="44"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="K8" s="47"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="46"/>
+      <c r="N8" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="O8" s="20"/>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="20"/>
-      <c r="R8" s="25"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="26"/>
+      <c r="R8" s="27"/>
       <c r="T8" s="7"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -1352,23 +1357,23 @@
       <c r="C9" s="3">
         <v>7</v>
       </c>
-      <c r="D9" s="40"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
-      <c r="N9" s="24" t="s">
+      <c r="D9" s="48"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="20"/>
-      <c r="R9" s="25"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="26"/>
+      <c r="Q9" s="26"/>
+      <c r="R9" s="27"/>
       <c r="U9" s="7"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
@@ -1381,21 +1386,21 @@
       <c r="C10" s="3">
         <v>8</v>
       </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="27"/>
-      <c r="N10" s="24"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="20"/>
-      <c r="R10" s="25"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="26"/>
+      <c r="P10" s="26"/>
+      <c r="Q10" s="26"/>
+      <c r="R10" s="27"/>
       <c r="U10" s="7"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -1408,23 +1413,23 @@
       <c r="C11" s="3">
         <v>9</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27"/>
-      <c r="N11" s="24" t="s">
+      <c r="D11" s="29"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="O11" s="20"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="20"/>
-      <c r="R11" s="25"/>
+      <c r="O11" s="26"/>
+      <c r="P11" s="26"/>
+      <c r="Q11" s="26"/>
+      <c r="R11" s="27"/>
       <c r="U11" s="7"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -1437,21 +1442,21 @@
       <c r="C12" s="3">
         <v>10</v>
       </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="27"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="20"/>
-      <c r="R12" s="25"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="26"/>
+      <c r="Q12" s="26"/>
+      <c r="R12" s="27"/>
       <c r="T12" s="7"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
@@ -1464,23 +1469,23 @@
       <c r="C13" s="3">
         <v>11</v>
       </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="42" t="s">
+      <c r="D13" s="29"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="K13" s="42"/>
-      <c r="L13" s="42"/>
-      <c r="M13" s="43"/>
-      <c r="N13" s="24"/>
-      <c r="O13" s="20"/>
-      <c r="P13" s="20"/>
-      <c r="Q13" s="20"/>
-      <c r="R13" s="25"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="42"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="26"/>
+      <c r="P13" s="26"/>
+      <c r="Q13" s="26"/>
+      <c r="R13" s="27"/>
       <c r="U13" s="7"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -1493,25 +1498,25 @@
       <c r="C14" s="3">
         <v>12</v>
       </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="42" t="s">
+      <c r="D14" s="29"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="M14" s="43"/>
-      <c r="N14" s="24" t="s">
+      <c r="M14" s="42"/>
+      <c r="N14" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="O14" s="20"/>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="20"/>
-      <c r="R14" s="25"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="26"/>
+      <c r="Q14" s="26"/>
+      <c r="R14" s="27"/>
       <c r="V14" s="7"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
@@ -1524,25 +1529,25 @@
       <c r="C15" s="3">
         <v>13</v>
       </c>
-      <c r="D15" s="44" t="s">
+      <c r="D15" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="42"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="27"/>
-      <c r="N15" s="24" t="s">
+      <c r="E15" s="41"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="O15" s="20"/>
-      <c r="P15" s="20"/>
-      <c r="Q15" s="20"/>
-      <c r="R15" s="25"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="26"/>
+      <c r="Q15" s="26"/>
+      <c r="R15" s="27"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -1554,23 +1559,23 @@
       <c r="C16" s="3">
         <v>14</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="27"/>
-      <c r="N16" s="24" t="s">
+      <c r="D16" s="29"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="O16" s="20"/>
-      <c r="P16" s="20"/>
-      <c r="Q16" s="20"/>
-      <c r="R16" s="25"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="26"/>
+      <c r="Q16" s="26"/>
+      <c r="R16" s="27"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -1582,23 +1587,23 @@
       <c r="C17" s="3">
         <v>15</v>
       </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="24" t="s">
+      <c r="D17" s="29"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="O17" s="20"/>
-      <c r="P17" s="20"/>
-      <c r="Q17" s="20"/>
-      <c r="R17" s="25"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
+      <c r="Q17" s="26"/>
+      <c r="R17" s="27"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
@@ -1610,23 +1615,23 @@
       <c r="C18" s="3">
         <v>16</v>
       </c>
-      <c r="D18" s="26"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="27"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="27"/>
-      <c r="N18" s="24" t="s">
+      <c r="D18" s="29"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="O18" s="20"/>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="20"/>
-      <c r="R18" s="25"/>
+      <c r="O18" s="26"/>
+      <c r="P18" s="26"/>
+      <c r="Q18" s="26"/>
+      <c r="R18" s="27"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -1638,21 +1643,21 @@
       <c r="C19" s="3">
         <v>17</v>
       </c>
-      <c r="D19" s="40"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="41"/>
-      <c r="L19" s="50"/>
-      <c r="M19" s="50"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="20"/>
-      <c r="R19" s="25"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="32"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="25"/>
+      <c r="O19" s="26"/>
+      <c r="P19" s="26"/>
+      <c r="Q19" s="26"/>
+      <c r="R19" s="27"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
@@ -1664,21 +1669,21 @@
       <c r="C20" s="3">
         <v>18</v>
       </c>
-      <c r="D20" s="40"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="41"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="41"/>
-      <c r="N20" s="24"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="20"/>
-      <c r="R20" s="25"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="25"/>
+      <c r="O20" s="26"/>
+      <c r="P20" s="26"/>
+      <c r="Q20" s="26"/>
+      <c r="R20" s="27"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
@@ -1690,21 +1695,21 @@
       <c r="C21" s="3">
         <v>19</v>
       </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="27"/>
-      <c r="N21" s="24"/>
-      <c r="O21" s="20"/>
-      <c r="P21" s="20"/>
-      <c r="Q21" s="20"/>
-      <c r="R21" s="25"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="25"/>
+      <c r="O21" s="26"/>
+      <c r="P21" s="26"/>
+      <c r="Q21" s="26"/>
+      <c r="R21" s="27"/>
     </row>
     <row r="22" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13">
@@ -1716,23 +1721,23 @@
       <c r="C22" s="14">
         <v>20</v>
       </c>
-      <c r="D22" s="45"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="46"/>
-      <c r="K22" s="46"/>
-      <c r="L22" s="46"/>
-      <c r="M22" s="47"/>
-      <c r="N22" s="51" t="s">
+      <c r="D22" s="36"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="38"/>
+      <c r="N22" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="O22" s="52"/>
-      <c r="P22" s="52"/>
-      <c r="Q22" s="52"/>
-      <c r="R22" s="53"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="20"/>
+      <c r="R22" s="21"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -1744,33 +1749,33 @@
       <c r="C23" s="3">
         <v>21</v>
       </c>
-      <c r="D23" s="48" t="s">
+      <c r="D23" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49" t="s">
+      <c r="E23" s="40"/>
+      <c r="F23" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49" t="s">
+      <c r="G23" s="40"/>
+      <c r="H23" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49" t="s">
+      <c r="I23" s="40"/>
+      <c r="J23" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="K23" s="49"/>
-      <c r="L23" s="49" t="s">
+      <c r="K23" s="40"/>
+      <c r="L23" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="M23" s="49"/>
-      <c r="N23" s="54" t="s">
+      <c r="M23" s="40"/>
+      <c r="N23" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="O23" s="55"/>
-      <c r="P23" s="55"/>
-      <c r="Q23" s="55"/>
-      <c r="R23" s="56"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="23"/>
+      <c r="Q23" s="23"/>
+      <c r="R23" s="24"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
@@ -1782,23 +1787,23 @@
       <c r="C24" s="3">
         <v>22</v>
       </c>
-      <c r="D24" s="29"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="30"/>
-      <c r="J24" s="30"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="30"/>
-      <c r="M24" s="30"/>
-      <c r="N24" s="21" t="s">
+      <c r="D24" s="34"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="35"/>
+      <c r="K24" s="35"/>
+      <c r="L24" s="35"/>
+      <c r="M24" s="35"/>
+      <c r="N24" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="O24" s="22"/>
-      <c r="P24" s="22"/>
-      <c r="Q24" s="22"/>
-      <c r="R24" s="23"/>
+      <c r="O24" s="54"/>
+      <c r="P24" s="54"/>
+      <c r="Q24" s="54"/>
+      <c r="R24" s="55"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
@@ -1810,21 +1815,21 @@
       <c r="C25" s="9">
         <v>23</v>
       </c>
-      <c r="D25" s="26"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="27"/>
-      <c r="L25" s="27"/>
-      <c r="M25" s="27"/>
-      <c r="N25" s="24"/>
-      <c r="O25" s="20"/>
-      <c r="P25" s="20"/>
-      <c r="Q25" s="20"/>
-      <c r="R25" s="25"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="30"/>
+      <c r="L25" s="30"/>
+      <c r="M25" s="30"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="26"/>
+      <c r="P25" s="26"/>
+      <c r="Q25" s="26"/>
+      <c r="R25" s="27"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
@@ -1836,21 +1841,21 @@
       <c r="C26" s="9">
         <v>24</v>
       </c>
-      <c r="D26" s="29"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="30"/>
-      <c r="J26" s="30"/>
-      <c r="K26" s="30"/>
-      <c r="L26" s="30"/>
-      <c r="M26" s="30"/>
-      <c r="N26" s="24"/>
-      <c r="O26" s="20"/>
-      <c r="P26" s="20"/>
-      <c r="Q26" s="20"/>
-      <c r="R26" s="25"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="35"/>
+      <c r="L26" s="35"/>
+      <c r="M26" s="35"/>
+      <c r="N26" s="25"/>
+      <c r="O26" s="26"/>
+      <c r="P26" s="26"/>
+      <c r="Q26" s="26"/>
+      <c r="R26" s="27"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
@@ -1862,21 +1867,21 @@
       <c r="C27" s="9">
         <v>25</v>
       </c>
-      <c r="D27" s="26"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="27"/>
-      <c r="K27" s="27"/>
-      <c r="L27" s="27"/>
-      <c r="M27" s="27"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="20"/>
-      <c r="P27" s="20"/>
-      <c r="Q27" s="20"/>
-      <c r="R27" s="25"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="25"/>
+      <c r="O27" s="26"/>
+      <c r="P27" s="26"/>
+      <c r="Q27" s="26"/>
+      <c r="R27" s="27"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
@@ -1888,57 +1893,130 @@
       <c r="C28" s="15">
         <v>26</v>
       </c>
-      <c r="D28" s="26"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="27"/>
-      <c r="K28" s="27"/>
-      <c r="L28" s="27"/>
-      <c r="M28" s="28"/>
-      <c r="N28" s="20"/>
-      <c r="O28" s="20"/>
-      <c r="P28" s="20"/>
-      <c r="Q28" s="20"/>
-      <c r="R28" s="25"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
+      <c r="K28" s="30"/>
+      <c r="L28" s="30"/>
+      <c r="M28" s="56"/>
+      <c r="N28" s="26"/>
+      <c r="O28" s="26"/>
+      <c r="P28" s="26"/>
+      <c r="Q28" s="26"/>
+      <c r="R28" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="163">
-    <mergeCell ref="N22:R22"/>
-    <mergeCell ref="N23:R23"/>
-    <mergeCell ref="N13:R13"/>
-    <mergeCell ref="N14:R14"/>
-    <mergeCell ref="N15:R15"/>
-    <mergeCell ref="N16:R16"/>
-    <mergeCell ref="N17:R17"/>
-    <mergeCell ref="N18:R18"/>
-    <mergeCell ref="N7:R7"/>
-    <mergeCell ref="N8:R8"/>
-    <mergeCell ref="N9:R9"/>
-    <mergeCell ref="N10:R10"/>
-    <mergeCell ref="N11:R11"/>
-    <mergeCell ref="N12:R12"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="N19:R19"/>
-    <mergeCell ref="N20:R20"/>
-    <mergeCell ref="N21:R21"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="N24:R24"/>
+    <mergeCell ref="N25:R25"/>
+    <mergeCell ref="N26:R26"/>
+    <mergeCell ref="N27:R27"/>
+    <mergeCell ref="N28:R28"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:M13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="L17:M17"/>
     <mergeCell ref="N2:R2"/>
     <mergeCell ref="N3:R3"/>
     <mergeCell ref="N4:R4"/>
@@ -1963,112 +2041,39 @@
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="J20:K20"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:M13"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="N24:R24"/>
-    <mergeCell ref="N25:R25"/>
-    <mergeCell ref="N26:R26"/>
-    <mergeCell ref="N27:R27"/>
-    <mergeCell ref="N28:R28"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="N19:R19"/>
+    <mergeCell ref="N20:R20"/>
+    <mergeCell ref="N21:R21"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="N22:R22"/>
+    <mergeCell ref="N23:R23"/>
+    <mergeCell ref="N13:R13"/>
+    <mergeCell ref="N14:R14"/>
+    <mergeCell ref="N15:R15"/>
+    <mergeCell ref="N16:R16"/>
+    <mergeCell ref="N17:R17"/>
+    <mergeCell ref="N18:R18"/>
+    <mergeCell ref="N7:R7"/>
+    <mergeCell ref="N8:R8"/>
+    <mergeCell ref="N9:R9"/>
+    <mergeCell ref="N10:R10"/>
+    <mergeCell ref="N11:R11"/>
+    <mergeCell ref="N12:R12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
handleiding en tekst voor presentatie
</commit_message>
<xml_diff>
--- a/Algemeen/Planning.xlsx
+++ b/Algemeen/Planning.xlsx
@@ -172,7 +172,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>Week</t>
   </si>
@@ -304,6 +304,12 @@
   </si>
   <si>
     <t>Ziek; maagklachten tot zondag</t>
+  </si>
+  <si>
+    <t>Deadline pdump</t>
+  </si>
+  <si>
+    <t>Presentatie op school</t>
   </si>
 </sst>
 </file>
@@ -360,7 +366,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -391,6 +397,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="23">
     <border>
@@ -650,7 +662,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -675,6 +687,117 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -692,114 +815,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1104,8 +1119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12:I12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,15 +1129,15 @@
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="55"/>
-      <c r="E1" s="27" t="s">
+      <c r="D1" s="20"/>
+      <c r="E1" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
@@ -1174,27 +1189,27 @@
       <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46" t="s">
+      <c r="D3" s="35"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46" t="s">
+      <c r="G3" s="36"/>
+      <c r="H3" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="26" t="s">
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="27"/>
-      <c r="R3" s="28"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="26"/>
       <c r="T3" s="10"/>
       <c r="U3" t="s">
         <v>29</v>
@@ -1210,29 +1225,29 @@
       <c r="C4" s="3">
         <v>2</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="46"/>
-      <c r="F4" s="49" t="s">
+      <c r="E4" s="36"/>
+      <c r="F4" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="49"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46" t="s">
+      <c r="G4" s="37"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="46"/>
-      <c r="N4" s="26" t="s">
+      <c r="M4" s="36"/>
+      <c r="N4" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="27"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="28"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="26"/>
       <c r="T4" s="11"/>
       <c r="U4" t="s">
         <v>30</v>
@@ -1248,25 +1263,25 @@
       <c r="C5" s="3">
         <v>3</v>
       </c>
-      <c r="D5" s="45"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="54" t="s">
+      <c r="D5" s="35"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="54"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="46"/>
-      <c r="N5" s="26" t="s">
+      <c r="I5" s="38"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="O5" s="27"/>
-      <c r="P5" s="27"/>
-      <c r="Q5" s="27"/>
-      <c r="R5" s="28"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="26"/>
       <c r="T5" s="16"/>
       <c r="U5" t="s">
         <v>31</v>
@@ -1282,23 +1297,23 @@
       <c r="C6" s="3">
         <v>4</v>
       </c>
-      <c r="D6" s="45"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="49" t="s">
+      <c r="D6" s="35"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="49"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="27"/>
-      <c r="P6" s="27"/>
-      <c r="Q6" s="27"/>
-      <c r="R6" s="28"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="21"/>
+      <c r="R6" s="26"/>
       <c r="T6" s="17"/>
       <c r="U6" s="15"/>
       <c r="V6" s="15"/>
@@ -1313,23 +1328,23 @@
       <c r="C7" s="12">
         <v>5</v>
       </c>
-      <c r="D7" s="52"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="46"/>
-      <c r="M7" s="46"/>
-      <c r="N7" s="26" t="s">
+      <c r="D7" s="39"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="36"/>
+      <c r="N7" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="O7" s="27"/>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="27"/>
-      <c r="R7" s="28"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="26"/>
       <c r="U7" s="7"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -1342,25 +1357,25 @@
       <c r="C8" s="3">
         <v>6</v>
       </c>
-      <c r="D8" s="47"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="49" t="s">
+      <c r="D8" s="41"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="K8" s="49"/>
-      <c r="L8" s="46"/>
-      <c r="M8" s="46"/>
-      <c r="N8" s="26" t="s">
+      <c r="K8" s="37"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="O8" s="27"/>
-      <c r="P8" s="27"/>
-      <c r="Q8" s="27"/>
-      <c r="R8" s="28"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="26"/>
       <c r="T8" s="7"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -1373,25 +1388,25 @@
       <c r="C9" s="3">
         <v>7</v>
       </c>
-      <c r="D9" s="45"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
-      <c r="J9" s="50" t="s">
+      <c r="D9" s="35"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="K9" s="50"/>
-      <c r="L9" s="50"/>
-      <c r="M9" s="51"/>
-      <c r="N9" s="26" t="s">
+      <c r="K9" s="43"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="44"/>
+      <c r="N9" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="O9" s="27"/>
-      <c r="P9" s="27"/>
-      <c r="Q9" s="27"/>
-      <c r="R9" s="28"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="26"/>
       <c r="U9" s="7"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
@@ -1404,21 +1419,23 @@
       <c r="C10" s="3">
         <v>8</v>
       </c>
-      <c r="D10" s="45"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="27"/>
-      <c r="P10" s="27"/>
-      <c r="Q10" s="27"/>
-      <c r="R10" s="28"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="M10" s="36"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="26"/>
       <c r="U10" s="7"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -1431,23 +1448,25 @@
       <c r="C11" s="3">
         <v>9</v>
       </c>
-      <c r="D11" s="30"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="26" t="s">
+      <c r="D11" s="35"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="K11" s="45"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="O11" s="27"/>
-      <c r="P11" s="27"/>
-      <c r="Q11" s="27"/>
-      <c r="R11" s="28"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="21"/>
+      <c r="R11" s="26"/>
       <c r="U11" s="7"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -1460,21 +1479,21 @@
       <c r="C12" s="3">
         <v>10</v>
       </c>
-      <c r="D12" s="30"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="27"/>
-      <c r="P12" s="27"/>
-      <c r="Q12" s="27"/>
-      <c r="R12" s="28"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="26"/>
       <c r="T12" s="7"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
@@ -1487,23 +1506,23 @@
       <c r="C13" s="3">
         <v>11</v>
       </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="42" t="s">
+      <c r="D13" s="29"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="K13" s="42"/>
-      <c r="L13" s="42"/>
-      <c r="M13" s="43"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="27"/>
-      <c r="R13" s="28"/>
+      <c r="K13" s="46"/>
+      <c r="L13" s="46"/>
+      <c r="M13" s="47"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="26"/>
       <c r="U13" s="7"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -1516,25 +1535,25 @@
       <c r="C14" s="3">
         <v>12</v>
       </c>
-      <c r="D14" s="30"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="42" t="s">
+      <c r="D14" s="29"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="M14" s="43"/>
-      <c r="N14" s="26" t="s">
+      <c r="M14" s="47"/>
+      <c r="N14" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="O14" s="27"/>
-      <c r="P14" s="27"/>
-      <c r="Q14" s="27"/>
-      <c r="R14" s="28"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="26"/>
       <c r="V14" s="7"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
@@ -1547,25 +1566,25 @@
       <c r="C15" s="3">
         <v>13</v>
       </c>
-      <c r="D15" s="44" t="s">
+      <c r="D15" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="42"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="31"/>
-      <c r="L15" s="31"/>
-      <c r="M15" s="31"/>
-      <c r="N15" s="26" t="s">
+      <c r="E15" s="46"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="O15" s="27"/>
-      <c r="P15" s="27"/>
-      <c r="Q15" s="27"/>
-      <c r="R15" s="28"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="21"/>
+      <c r="R15" s="26"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -1577,23 +1596,23 @@
       <c r="C16" s="3">
         <v>14</v>
       </c>
-      <c r="D16" s="30"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="31"/>
-      <c r="L16" s="31"/>
-      <c r="M16" s="31"/>
-      <c r="N16" s="26" t="s">
+      <c r="D16" s="29"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="O16" s="27"/>
-      <c r="P16" s="27"/>
-      <c r="Q16" s="27"/>
-      <c r="R16" s="28"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="21"/>
+      <c r="Q16" s="21"/>
+      <c r="R16" s="26"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -1605,23 +1624,23 @@
       <c r="C17" s="3">
         <v>15</v>
       </c>
-      <c r="D17" s="30"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="31"/>
-      <c r="N17" s="26" t="s">
+      <c r="D17" s="29"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="O17" s="27"/>
-      <c r="P17" s="27"/>
-      <c r="Q17" s="27"/>
-      <c r="R17" s="28"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="21"/>
+      <c r="Q17" s="21"/>
+      <c r="R17" s="26"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
@@ -1633,23 +1652,23 @@
       <c r="C18" s="3">
         <v>16</v>
       </c>
-      <c r="D18" s="30"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="26" t="s">
+      <c r="D18" s="29"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="O18" s="27"/>
-      <c r="P18" s="27"/>
-      <c r="Q18" s="27"/>
-      <c r="R18" s="28"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="26"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -1661,21 +1680,21 @@
       <c r="C19" s="3">
         <v>17</v>
       </c>
-      <c r="D19" s="32"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="27"/>
-      <c r="P19" s="27"/>
-      <c r="Q19" s="27"/>
-      <c r="R19" s="28"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="55"/>
+      <c r="H19" s="55"/>
+      <c r="I19" s="55"/>
+      <c r="J19" s="55"/>
+      <c r="K19" s="55"/>
+      <c r="L19" s="56"/>
+      <c r="M19" s="56"/>
+      <c r="N19" s="25"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="26"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
@@ -1687,21 +1706,21 @@
       <c r="C20" s="3">
         <v>18</v>
       </c>
-      <c r="D20" s="32"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="29"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="26"/>
-      <c r="O20" s="27"/>
-      <c r="P20" s="27"/>
-      <c r="Q20" s="27"/>
-      <c r="R20" s="28"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="55"/>
+      <c r="J20" s="55"/>
+      <c r="K20" s="55"/>
+      <c r="L20" s="55"/>
+      <c r="M20" s="55"/>
+      <c r="N20" s="25"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="21"/>
+      <c r="Q20" s="21"/>
+      <c r="R20" s="26"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
@@ -1713,21 +1732,21 @@
       <c r="C21" s="3">
         <v>19</v>
       </c>
-      <c r="D21" s="30"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="31"/>
-      <c r="L21" s="31"/>
-      <c r="M21" s="31"/>
-      <c r="N21" s="26"/>
-      <c r="O21" s="27"/>
-      <c r="P21" s="27"/>
-      <c r="Q21" s="27"/>
-      <c r="R21" s="28"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="25"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="21"/>
+      <c r="Q21" s="21"/>
+      <c r="R21" s="26"/>
     </row>
     <row r="22" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13">
@@ -1739,23 +1758,23 @@
       <c r="C22" s="14">
         <v>20</v>
       </c>
-      <c r="D22" s="37"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="38"/>
-      <c r="L22" s="38"/>
-      <c r="M22" s="39"/>
-      <c r="N22" s="20" t="s">
+      <c r="D22" s="49"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="50"/>
+      <c r="H22" s="50"/>
+      <c r="I22" s="50"/>
+      <c r="J22" s="50"/>
+      <c r="K22" s="50"/>
+      <c r="L22" s="50"/>
+      <c r="M22" s="51"/>
+      <c r="N22" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="O22" s="21"/>
-      <c r="P22" s="21"/>
-      <c r="Q22" s="21"/>
-      <c r="R22" s="22"/>
+      <c r="O22" s="58"/>
+      <c r="P22" s="58"/>
+      <c r="Q22" s="58"/>
+      <c r="R22" s="59"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -1767,33 +1786,33 @@
       <c r="C23" s="3">
         <v>21</v>
       </c>
-      <c r="D23" s="40" t="s">
+      <c r="D23" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41" t="s">
+      <c r="E23" s="53"/>
+      <c r="F23" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="G23" s="41"/>
-      <c r="H23" s="41" t="s">
+      <c r="G23" s="53"/>
+      <c r="H23" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="I23" s="41"/>
-      <c r="J23" s="41" t="s">
+      <c r="I23" s="53"/>
+      <c r="J23" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="K23" s="41"/>
-      <c r="L23" s="41" t="s">
+      <c r="K23" s="53"/>
+      <c r="L23" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="M23" s="41"/>
-      <c r="N23" s="23" t="s">
+      <c r="M23" s="53"/>
+      <c r="N23" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="O23" s="24"/>
-      <c r="P23" s="24"/>
-      <c r="Q23" s="24"/>
-      <c r="R23" s="25"/>
+      <c r="O23" s="61"/>
+      <c r="P23" s="61"/>
+      <c r="Q23" s="61"/>
+      <c r="R23" s="62"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
@@ -1805,23 +1824,23 @@
       <c r="C24" s="3">
         <v>22</v>
       </c>
-      <c r="D24" s="35"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="36"/>
-      <c r="K24" s="36"/>
-      <c r="L24" s="36"/>
-      <c r="M24" s="36"/>
-      <c r="N24" s="56" t="s">
+      <c r="D24" s="31"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="32"/>
+      <c r="N24" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="O24" s="57"/>
-      <c r="P24" s="57"/>
-      <c r="Q24" s="57"/>
-      <c r="R24" s="58"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="23"/>
+      <c r="Q24" s="23"/>
+      <c r="R24" s="24"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
@@ -1833,21 +1852,21 @@
       <c r="C25" s="9">
         <v>23</v>
       </c>
-      <c r="D25" s="30"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="31"/>
-      <c r="M25" s="31"/>
-      <c r="N25" s="26"/>
-      <c r="O25" s="27"/>
-      <c r="P25" s="27"/>
-      <c r="Q25" s="27"/>
-      <c r="R25" s="28"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="30"/>
+      <c r="L25" s="30"/>
+      <c r="M25" s="30"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="21"/>
+      <c r="Q25" s="21"/>
+      <c r="R25" s="26"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
@@ -1859,21 +1878,21 @@
       <c r="C26" s="9">
         <v>24</v>
       </c>
-      <c r="D26" s="35"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="36"/>
-      <c r="K26" s="36"/>
-      <c r="L26" s="36"/>
-      <c r="M26" s="36"/>
-      <c r="N26" s="26"/>
-      <c r="O26" s="27"/>
-      <c r="P26" s="27"/>
-      <c r="Q26" s="27"/>
-      <c r="R26" s="28"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="32"/>
+      <c r="N26" s="25"/>
+      <c r="O26" s="21"/>
+      <c r="P26" s="21"/>
+      <c r="Q26" s="21"/>
+      <c r="R26" s="26"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
@@ -1885,21 +1904,21 @@
       <c r="C27" s="9">
         <v>25</v>
       </c>
-      <c r="D27" s="30"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="31"/>
-      <c r="L27" s="31"/>
-      <c r="M27" s="31"/>
-      <c r="N27" s="26"/>
-      <c r="O27" s="27"/>
-      <c r="P27" s="27"/>
-      <c r="Q27" s="27"/>
-      <c r="R27" s="28"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="25"/>
+      <c r="O27" s="21"/>
+      <c r="P27" s="21"/>
+      <c r="Q27" s="21"/>
+      <c r="R27" s="26"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="18">
@@ -1911,24 +1930,162 @@
       <c r="C28" s="4">
         <v>26</v>
       </c>
-      <c r="D28" s="35"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
-      <c r="K28" s="36"/>
-      <c r="L28" s="36"/>
-      <c r="M28" s="61"/>
-      <c r="N28" s="59"/>
-      <c r="O28" s="59"/>
-      <c r="P28" s="59"/>
-      <c r="Q28" s="59"/>
-      <c r="R28" s="60"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="32"/>
+      <c r="L28" s="32"/>
+      <c r="M28" s="33"/>
+      <c r="N28" s="27"/>
+      <c r="O28" s="27"/>
+      <c r="P28" s="27"/>
+      <c r="Q28" s="27"/>
+      <c r="R28" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="162">
+    <mergeCell ref="N22:R22"/>
+    <mergeCell ref="N23:R23"/>
+    <mergeCell ref="N13:R13"/>
+    <mergeCell ref="N14:R14"/>
+    <mergeCell ref="N15:R15"/>
+    <mergeCell ref="N16:R16"/>
+    <mergeCell ref="N17:R17"/>
+    <mergeCell ref="N18:R18"/>
+    <mergeCell ref="N7:R7"/>
+    <mergeCell ref="N8:R8"/>
+    <mergeCell ref="N9:R9"/>
+    <mergeCell ref="N10:R10"/>
+    <mergeCell ref="N11:R11"/>
+    <mergeCell ref="N12:R12"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="N19:R19"/>
+    <mergeCell ref="N20:R20"/>
+    <mergeCell ref="N21:R21"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="N3:R3"/>
+    <mergeCell ref="N4:R4"/>
+    <mergeCell ref="N5:R5"/>
+    <mergeCell ref="N6:R6"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:M13"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="D6:E6"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="N24:R24"/>
@@ -1953,144 +2110,6 @@
     <mergeCell ref="L25:M25"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="F26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:M9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:M13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="N2:R2"/>
-    <mergeCell ref="N3:R3"/>
-    <mergeCell ref="N4:R4"/>
-    <mergeCell ref="N5:R5"/>
-    <mergeCell ref="N6:R6"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="N19:R19"/>
-    <mergeCell ref="N20:R20"/>
-    <mergeCell ref="N21:R21"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="N22:R22"/>
-    <mergeCell ref="N23:R23"/>
-    <mergeCell ref="N13:R13"/>
-    <mergeCell ref="N14:R14"/>
-    <mergeCell ref="N15:R15"/>
-    <mergeCell ref="N16:R16"/>
-    <mergeCell ref="N17:R17"/>
-    <mergeCell ref="N18:R18"/>
-    <mergeCell ref="N7:R7"/>
-    <mergeCell ref="N8:R8"/>
-    <mergeCell ref="N9:R9"/>
-    <mergeCell ref="N10:R10"/>
-    <mergeCell ref="N11:R11"/>
-    <mergeCell ref="N12:R12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>